<commit_message>
Update Team01Report-Sprint4 - End of Project.xlsx
</commit_message>
<xml_diff>
--- a/docs/Team01Report-Sprint4 - End of Project.xlsx
+++ b/docs/Team01Report-Sprint4 - End of Project.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="271">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -854,6 +854,33 @@
   </si>
   <si>
     <t>Bug found in gedcom main</t>
+  </si>
+  <si>
+    <t>Check Dates</t>
+  </si>
+  <si>
+    <t>Loop Ages and check is 2x</t>
+  </si>
+  <si>
+    <t>Loop all INDI</t>
+  </si>
+  <si>
+    <t>Last last name of males</t>
+  </si>
+  <si>
+    <t>Print Bdays for upcomming</t>
+  </si>
+  <si>
+    <t>Loops all INDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Fam </t>
+  </si>
+  <si>
+    <t>Check if Death of botharents</t>
+  </si>
+  <si>
+    <t>Check recent deaths</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1036,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1042,6 +1069,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1212,11 +1240,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="454164304"/>
-        <c:axId val="454166656"/>
+        <c:axId val="405699584"/>
+        <c:axId val="405699976"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="454164304"/>
+        <c:axId val="405699584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,14 +1254,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454166656"/>
+        <c:crossAx val="405699976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="454166656"/>
+        <c:axId val="405699976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,7 +1272,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454164304"/>
+        <c:crossAx val="405699584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1349,11 +1377,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="454163128"/>
-        <c:axId val="454165480"/>
+        <c:axId val="405696840"/>
+        <c:axId val="405702720"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="454163128"/>
+        <c:axId val="405696840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,14 +1391,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454165480"/>
+        <c:crossAx val="405702720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="454165480"/>
+        <c:axId val="405702720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454163128"/>
+        <c:crossAx val="405696840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1418,7 +1446,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,7 +1484,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1531,7 +1559,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1596,7 +1624,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1665,7 +1693,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1735,7 +1763,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1804,7 +1832,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1874,7 +1902,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3453,7 +3481,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H27"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3926,8 +3954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B40"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4412,10 +4440,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4453,296 +4481,469 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="17">
         <v>50</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="17">
         <v>45</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="17">
         <v>49</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="17">
         <v>45</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="22" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>0.01</v>
+      </c>
+      <c r="B3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.02</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3">
+      <c r="D5" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="17">
         <v>60</v>
       </c>
-      <c r="F3">
+      <c r="F5" s="17">
         <v>50</v>
       </c>
-      <c r="G3">
+      <c r="G5" s="17">
         <v>80</v>
       </c>
-      <c r="H3">
+      <c r="H5" s="17">
         <v>60</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I5" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.01</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.02</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4">
+      <c r="D8" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="17">
         <v>50</v>
       </c>
-      <c r="F4">
+      <c r="F8" s="17">
         <v>45</v>
       </c>
-      <c r="G4">
+      <c r="G8" s="17">
         <v>53</v>
       </c>
-      <c r="H4">
+      <c r="H8" s="17">
         <v>45</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="I8" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.01</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.02</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C11" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5">
+      <c r="D11" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="17">
         <v>30</v>
       </c>
-      <c r="F5">
+      <c r="F11" s="17">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G11" s="17">
         <v>52</v>
       </c>
-      <c r="H5">
+      <c r="H11" s="17">
         <v>50</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="I11" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.01</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.02</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B14" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C14" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6">
+      <c r="D14" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="17">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="F14" s="17">
         <v>20</v>
       </c>
-      <c r="G6">
+      <c r="G14" s="17">
         <v>52</v>
       </c>
-      <c r="H6">
+      <c r="H14" s="17">
         <v>40</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="I14" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.01</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.02</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B17" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C17" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7">
+      <c r="D17" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="17">
         <v>40</v>
       </c>
-      <c r="F7">
+      <c r="F17" s="17">
         <v>40</v>
       </c>
-      <c r="G7">
+      <c r="G17" s="17">
         <v>58</v>
       </c>
-      <c r="H7">
+      <c r="H17" s="17">
         <v>30</v>
       </c>
-      <c r="I7" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="I17" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.01</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.02</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B20" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C20" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8">
+      <c r="D20" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="17">
         <v>50</v>
       </c>
-      <c r="F8">
+      <c r="F20" s="17">
         <v>35</v>
       </c>
-      <c r="G8">
+      <c r="G20" s="17">
         <v>64</v>
       </c>
-      <c r="H8">
+      <c r="H20" s="17">
         <v>35</v>
       </c>
-      <c r="I8" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="I20" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.01</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.02</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B23" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C23" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9">
+      <c r="D23" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="17">
         <v>45</v>
       </c>
-      <c r="F9">
+      <c r="F23" s="17">
         <v>40</v>
       </c>
-      <c r="G9">
+      <c r="G23" s="17">
         <v>73</v>
       </c>
-      <c r="H9">
+      <c r="H23" s="17">
         <v>55</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="18"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="I23" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.01</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0.02</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.03</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="21" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="18" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="18" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="18" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="18" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="20" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="18"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="20" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="18" t="s">
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="18" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="18" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="18" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="18" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="18" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="18" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="18" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5063,7 +5264,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>137</v>
       </c>

</xml_diff>